<commit_message>
added step for updated freeze patch info
</commit_message>
<xml_diff>
--- a/data/novelomics/rd3_novelomics.xlsx
+++ b/data/novelomics/rd3_novelomics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcruvolo/GitHub/molgenis-solve-rd/data/novelomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D313F40-E87E-9D41-B1DC-55AE148126B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B305097F-2D3C-494D-9E78-AD5D524AC1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-5140" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1311,8 +1311,8 @@
   <dimension ref="A1:X83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I74" sqref="I74"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1666,7 +1666,7 @@
         <v>240</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>56</v>

</xml_diff>